<commit_message>
comment test and lexer diagram
</commit_message>
<xml_diff>
--- a/docs/lexer STD.xlsx
+++ b/docs/lexer STD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\compiler assignment\compiler\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wayne\Desktop\cps2000 compiler\CPS2000-compiler\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB362937-616F-4AFA-A340-A6AC58551388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926E19E3-0A54-40D7-A0A6-A58D788185AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{3D1BC879-8A1E-42C0-A222-4C84FA46729B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D1BC879-8A1E-42C0-A222-4C84FA46729B}"/>
   </bookViews>
   <sheets>
     <sheet name="Classifier table" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="135">
   <si>
     <t>Class</t>
   </si>
@@ -450,6 +450,24 @@
   </si>
   <si>
     <t>arrow</t>
+  </si>
+  <si>
+    <t>NewLine</t>
+  </si>
+  <si>
+    <t>singeLineComment</t>
+  </si>
+  <si>
+    <t>multiLineComment</t>
+  </si>
+  <si>
+    <t>WhiteSpace</t>
+  </si>
+  <si>
+    <t>\r\f\n</t>
+  </si>
+  <si>
+    <t>Character.isWhitespace(c)</t>
   </si>
 </sst>
 </file>
@@ -497,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -506,6 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,18 +805,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO22"/>
+  <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -805,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -840,7 +859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -881,7 +900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -1006,7 +1025,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1014,7 +1033,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1022,7 +1041,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -1030,7 +1049,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -1038,7 +1057,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>106</v>
       </c>
@@ -1046,7 +1065,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1054,7 +1073,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -1062,7 +1081,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -1070,7 +1089,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1078,7 +1097,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -1086,7 +1105,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -1094,7 +1113,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -1102,7 +1121,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -1110,7 +1129,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -1118,7 +1137,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -1126,7 +1145,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -1134,7 +1153,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -1142,7 +1161,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>125</v>
       </c>
@@ -1150,7 +1169,31 @@
         <v>126</v>
       </c>
     </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B24:G24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1158,18 +1201,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D8FA0B-C8DD-41CF-B72E-6DD1ADF0D158}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>89</v>
       </c>
@@ -1180,22 +1223,22 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1203,7 +1246,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1211,12 +1254,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -1224,37 +1267,37 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -1262,7 +1305,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -1270,7 +1313,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -1278,7 +1321,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>108</v>
       </c>
@@ -1286,7 +1329,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1294,7 +1337,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -1302,7 +1345,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>119</v>
       </c>
@@ -1310,7 +1353,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -1318,7 +1361,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>121</v>
       </c>
@@ -1326,7 +1369,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>122</v>
       </c>
@@ -1334,7 +1377,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>115</v>
       </c>
@@ -1342,7 +1385,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>116</v>
       </c>
@@ -1350,7 +1393,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>117</v>
       </c>
@@ -1358,7 +1401,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>118</v>
       </c>
@@ -1366,7 +1409,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -1374,7 +1417,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -1382,7 +1425,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -1390,7 +1433,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -1398,7 +1441,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>123</v>
       </c>
@@ -1406,7 +1449,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>124</v>
       </c>
@@ -1414,7 +1457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>127</v>
       </c>
@@ -1422,11 +1465,27 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>128</v>
       </c>
       <c r="B36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1440,38 +1499,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1093112-F7B4-4E0D-B4D3-F650519D60B8}">
-  <dimension ref="A1:W37"/>
+  <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" customWidth="1"/>
-    <col min="4" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" customWidth="1"/>
+    <col min="4" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" customWidth="1"/>
     <col min="8" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1483,9 +1542,9 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="str" cm="1">
-        <f t="array" ref="C2:W2">TRANSPOSE(_xlfn._xlws.FILTER('Classifier table'!A2:A200,LEN('Classifier table'!A2:A200)&lt;&gt;0))</f>
+        <f t="array" ref="C2:Y2">TRANSPOSE(_xlfn._xlws.FILTER('Classifier table'!A2:A200,LEN('Classifier table'!A2:A200)&lt;&gt;0))</f>
         <v>Digit</v>
       </c>
       <c r="D2" s="1" t="str">
@@ -1548,13 +1607,19 @@
       <c r="W2" s="1" t="str">
         <v>Comma</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2" s="1" t="str">
+        <v>NewLine</v>
+      </c>
+      <c r="Y2" s="1" t="str">
+        <v>WhiteSpace</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B3" s="1" t="str" cm="1">
-        <f t="array" ref="B3:B37">_xlfn._xlws.FILTER(Tokens!A2:A208,LEN(Tokens!A2:A208)&lt;&gt;0)</f>
+        <f t="array" ref="B3:B39">_xlfn._xlws.FILTER(Tokens!A2:A208,LEN(Tokens!A2:A208)&lt;&gt;0)</f>
         <v>start</v>
       </c>
       <c r="C3" t="s">
@@ -1618,7 +1683,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="str">
         <v>under1</v>
@@ -1627,7 +1692,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="str">
         <v>under2</v>
@@ -1639,7 +1704,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="str">
         <v>sysFunc</v>
@@ -1651,7 +1716,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="str">
         <v>int</v>
@@ -1663,7 +1728,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="str">
         <v>intPoint</v>
@@ -1672,7 +1737,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="str">
         <v>float</v>
@@ -1681,7 +1746,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="str">
         <v>pound</v>
@@ -1693,7 +1758,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="str">
         <v>hex1</v>
@@ -1705,7 +1770,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="str">
         <v>hex2</v>
@@ -1717,7 +1782,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="str">
         <v>hex3</v>
@@ -1729,7 +1794,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="str">
         <v>hex4</v>
@@ -1741,7 +1806,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="str">
         <v>hex5</v>
@@ -1753,12 +1818,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="str">
         <v>colour</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="str">
         <v>word</v>
       </c>
@@ -1775,7 +1840,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="str">
         <v>equals</v>
       </c>
@@ -1783,7 +1848,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="str">
         <v>exclamation</v>
       </c>
@@ -1791,7 +1856,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="str">
         <v>GT</v>
       </c>
@@ -1799,7 +1864,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="str">
         <v>LT</v>
       </c>
@@ -1807,42 +1872,42 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="str">
         <v>EQ</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="str">
         <v>NE</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="str">
         <v>GTE</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="str">
         <v>LTE</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="str">
         <v>multiply</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="str">
         <v>divide</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="str">
         <v>add</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="str">
         <v>subtract</v>
       </c>
@@ -1850,44 +1915,54 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="str">
         <v>bracOpen</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="str">
         <v>bracClose</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="str">
         <v>curlyBracOpen</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="str">
         <v>curlyBracClose</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="str">
         <v>semiColon</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="str">
         <v>colon</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="str">
         <v>comma</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="str">
         <v>arrow</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="str">
+        <v>singeLineComment</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="str">
+        <v>multiLineComment</v>
       </c>
     </row>
   </sheetData>

</xml_diff>